<commit_message>
Added PDF showing 4 vCPU results
</commit_message>
<xml_diff>
--- a/docs/results_sheet_nginx_static_200_4vCPU.xlsx
+++ b/docs/results_sheet_nginx_static_200_4vCPU.xlsx
@@ -934,6 +934,30 @@
     </mc:Fallback>
   </mc:AlternateContent>
   <c:chart>
+    <c:title>
+      <c:tx>
+        <c:rich>
+          <a:bodyPr/>
+          <a:lstStyle/>
+          <a:p>
+            <a:pPr>
+              <a:defRPr/>
+            </a:pPr>
+            <a:r>
+              <a:rPr lang="en-US" sz="1800" b="1" i="0" baseline="0">
+                <a:effectLst/>
+              </a:rPr>
+              <a:t>Nginx with FPM, static pool = 200, 4vCPUs</a:t>
+            </a:r>
+            <a:endParaRPr lang="en-US">
+              <a:effectLst/>
+            </a:endParaRPr>
+          </a:p>
+        </c:rich>
+      </c:tx>
+      <c:layout/>
+      <c:overlay val="0"/>
+    </c:title>
     <c:autoTitleDeleted val="0"/>
     <c:plotArea>
       <c:layout/>
@@ -2954,11 +2978,11 @@
         </c:dLbls>
         <c:marker val="1"/>
         <c:smooth val="0"/>
-        <c:axId val="2102616984"/>
-        <c:axId val="2108840264"/>
+        <c:axId val="2146752680"/>
+        <c:axId val="2146764728"/>
       </c:lineChart>
       <c:catAx>
-        <c:axId val="2102616984"/>
+        <c:axId val="2146752680"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -2992,7 +3016,7 @@
         <c:majorTickMark val="out"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="2108840264"/>
+        <c:crossAx val="2146764728"/>
         <c:crosses val="autoZero"/>
         <c:auto val="1"/>
         <c:lblAlgn val="ctr"/>
@@ -3000,7 +3024,7 @@
         <c:noMultiLvlLbl val="0"/>
       </c:catAx>
       <c:valAx>
-        <c:axId val="2108840264"/>
+        <c:axId val="2146764728"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -3030,7 +3054,7 @@
         <c:majorTickMark val="out"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="2102616984"/>
+        <c:crossAx val="2146752680"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="between"/>
       </c:valAx>

</xml_diff>